<commit_message>
Non-energy use is no longer useful.
</commit_message>
<xml_diff>
--- a/inst/extdata/Machines - Data/Non-energy/Non-energy.xlsx
+++ b/inst/extdata/Machines - Data/Non-energy/Non-energy.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992222BC-831E-E84F-9FAC-8F9834214191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="3" r:id="rId1"/>
@@ -118,8 +119,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +153,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -183,7 +191,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -200,10 +208,16 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2 3" xfId="1"/>
+    <cellStyle name="Normal 2 2 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -480,21 +494,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" customWidth="1"/>
-    <col min="3" max="3" width="54.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" customWidth="1"/>
+    <col min="3" max="3" width="54.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -505,7 +519,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -516,7 +530,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -531,24 +545,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="H15" sqref="H15:H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -557,7 +571,7 @@
       <c r="D1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -586,7 +600,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -608,12 +622,12 @@
       <c r="G3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="8"/>
       <c r="I3" s="7">
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
@@ -635,11 +649,12 @@
       <c r="G4" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="H4" s="9"/>
       <c r="I4" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>16</v>
       </c>
@@ -668,7 +683,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
@@ -697,7 +712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
@@ -726,7 +741,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
@@ -755,7 +770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
@@ -777,11 +792,12 @@
       <c r="G9" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="H9" s="8"/>
       <c r="I9" s="7">
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -803,11 +819,12 @@
       <c r="G10" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="H10" s="9"/>
       <c r="I10" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
@@ -829,11 +846,12 @@
       <c r="G11" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="H11" s="8"/>
       <c r="I11" s="7">
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>15</v>
       </c>
@@ -855,11 +873,12 @@
       <c r="G12" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="H12" s="9"/>
       <c r="I12" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
@@ -884,8 +903,9 @@
       <c r="H13" s="7">
         <v>9.9999999999999995E-7</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
@@ -910,8 +930,9 @@
       <c r="H14" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
@@ -933,11 +954,12 @@
       <c r="G15" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="H15" s="8"/>
       <c r="I15" s="7">
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>16</v>
       </c>
@@ -959,11 +981,12 @@
       <c r="G16" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="H16" s="9"/>
       <c r="I16" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
@@ -985,11 +1008,12 @@
       <c r="G17" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="H17" s="8"/>
       <c r="I17" s="7">
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>16</v>
       </c>
@@ -1011,11 +1035,12 @@
       <c r="G18" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="H18" s="9"/>
       <c r="I18" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>16</v>
       </c>
@@ -1037,11 +1062,12 @@
       <c r="G19" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="H19" s="8"/>
       <c r="I19" s="7">
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>16</v>
       </c>
@@ -1063,41 +1089,51 @@
       <c r="G20" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="H20" s="9"/>
       <c r="I20" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010060B7F65646EC444FB25DA4F5E743F4A7" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d7f09569f4a64415a488fee814f89e9f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="77d41baf-5ecc-4842-ba36-0ed33caf7049" xmlns:ns4="83e0870f-5ab0-41af-b2c4-f358cb535498" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8efd8f378c7a4511217f3fc9a2a42926" ns3:_="" ns4:_="">
     <xsd:import namespace="77d41baf-5ecc-4842-ba36-0ed33caf7049"/>
@@ -1314,22 +1350,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D57BA165-9822-445B-B328-4F06AD982831}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F97C2014-63BC-4AD0-B7B7-B33C587EA9A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1348,7 +1383,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF083C1D-CE62-48EF-BAF9-9D27C80F6E5E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="77d41baf-5ecc-4842-ba36-0ed33caf7049"/>
@@ -1363,12 +1398,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D57BA165-9822-445B-B328-4F06AD982831}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>